<commit_message>
Updated dt1_chartscript data and chart titles
</commit_message>
<xml_diff>
--- a/gapMinder-DT1/data/GapMinder Validado.xlsx
+++ b/gapMinder-DT1/data/GapMinder Validado.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avelez/Desktop/PAAA/Excel Documets/Delitos Tipo 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avelez/Documents/GitHub/erduprojectarecibo.github.io/gapMinder-DT1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6ABC543C-40D2-E742-B3EE-235C9587F39D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F2B39B-5D8C-BC47-B042-7CB89721AAA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{1E8408A5-A65C-5141-B9E3-3A48FD0CEBF2}"/>
   </bookViews>
@@ -67,7 +67,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +87,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,10 +144,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -153,9 +161,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{7A77AAA1-FD51-9842-B032-874A53721C19}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -469,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D172E5B-3A9C-5B41-A7F7-B3127C515192}">
   <dimension ref="A1:F218"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1584,8 +1594,8 @@
       <c r="D65" s="3">
         <v>771</v>
       </c>
-      <c r="E65" s="4">
-        <v>2730.5</v>
+      <c r="E65" s="10">
+        <v>2760.0674883400629</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -1737,8 +1747,8 @@
       <c r="D74" s="3">
         <v>629.4</v>
       </c>
-      <c r="E74" s="4">
-        <v>2534.4</v>
+      <c r="E74" s="10">
+        <v>2539.6212774720725</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>